<commit_message>
June 2021 - Update
Minor update to correct a feature list error effecting F3 license types, plus some cosmetic improvements.
</commit_message>
<xml_diff>
--- a/Microsoft 365 License Matrix.xlsx
+++ b/Microsoft 365 License Matrix.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="707" documentId="13_ncr:40009_{1420BF28-4C29-4990-B2CC-D0D9EF7DD0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{585D8FBD-802A-452E-8BA9-3BD58740111B}"/>
+  <xr:revisionPtr revIDLastSave="782" documentId="13_ncr:40009_{1420BF28-4C29-4990-B2CC-D0D9EF7DD0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{050FECFD-B6EF-400F-8791-4E44F51C3675}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="393">
   <si>
     <t>Enterprise Mobility + Security</t>
   </si>
@@ -1201,6 +1201,21 @@
   </si>
   <si>
     <t>~</t>
+  </si>
+  <si>
+    <t>❌</t>
+  </si>
+  <si>
+    <t>Labels</t>
+  </si>
+  <si>
+    <t>Pro</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>~E3~</t>
   </si>
 </sst>
 </file>
@@ -1362,6 +1377,7 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2040,9 +2056,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2130,6 +2143,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2739,33 +2755,33 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.23046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.69140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.23046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.23046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.23046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.23046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="167.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="2" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" style="1" customWidth="1"/>
+    <col min="20" max="20" width="184.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="55">
-        <v>44362</v>
-      </c>
-      <c r="B1" s="66" t="s">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="54">
+        <v>44363</v>
+      </c>
+      <c r="B1" s="65" t="s">
         <v>302</v>
       </c>
       <c r="C1" s="78" t="s">
@@ -2794,11 +2810,11 @@
       <c r="R1" s="79"/>
       <c r="S1" s="80"/>
     </row>
-    <row r="2" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>281</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="66" t="s">
         <v>368</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2819,10 +2835,10 @@
       <c r="H2" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="55" t="s">
         <v>292</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="56" t="s">
         <v>385</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -2856,11 +2872,11 @@
         <v>280</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A3" s="51" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="50" t="s">
         <v>302</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="67" t="s">
         <v>368</v>
       </c>
       <c r="C3" s="8"/>
@@ -2894,11 +2910,11 @@
       </c>
       <c r="T3" s="10"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="59"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="13"/>
@@ -2933,11 +2949,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C5" s="12" t="s">
@@ -2984,11 +3000,11 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="59"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="13"/>
@@ -3017,11 +3033,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="B7" s="59"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="13"/>
@@ -3056,11 +3072,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -3107,11 +3123,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A9" s="48" t="s">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
         <v>275</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="62" t="s">
         <v>363</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -3158,11 +3174,11 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A10" s="48" t="s">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
         <v>372</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="62" t="s">
         <v>363</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -3182,7 +3198,7 @@
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="74" t="str">
+      <c r="J10" s="73" t="str">
         <f>IF(OR(Matrix[[#This Row],[F5 Security]]="✔",Matrix[[#This Row],[F5 Compliance]]="✔"),"✔","")</f>
         <v/>
       </c>
@@ -3205,15 +3221,15 @@
       <c r="S10" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="T10" s="54" t="s">
+      <c r="T10" s="53" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="59"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
         <v>363</v>
@@ -3250,11 +3266,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B12" s="59"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="13"/>
@@ -3289,11 +3305,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="59"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
@@ -3328,11 +3344,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="59"/>
+      <c r="B14" s="58"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="13"/>
@@ -3367,11 +3383,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="59"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="13" t="s">
@@ -3410,11 +3426,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B16" s="59"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="13"/>
@@ -3449,11 +3465,11 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B17" s="59"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="13"/>
@@ -3488,11 +3504,11 @@
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A18" s="50" t="s">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="49" t="s">
         <v>357</v>
       </c>
-      <c r="B18" s="59"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="13"/>
@@ -3527,11 +3543,11 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A19" s="50" t="s">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="49" t="s">
         <v>362</v>
       </c>
-      <c r="B19" s="59"/>
+      <c r="B19" s="58"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="13"/>
@@ -3570,11 +3586,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="69" t="s">
+      <c r="B20" s="68" t="s">
         <v>347</v>
       </c>
       <c r="C20" s="12" t="s">
@@ -3621,11 +3637,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A21" s="52" t="s">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="58" t="s">
         <v>383</v>
       </c>
       <c r="C21" s="12" t="s">
@@ -3669,11 +3685,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C22" s="12" t="s">
@@ -3718,11 +3734,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B23" s="59"/>
+      <c r="B23" s="58"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="13"/>
@@ -3751,11 +3767,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B24" s="59"/>
+      <c r="B24" s="58"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="13"/>
@@ -3790,11 +3806,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="59"/>
+      <c r="B25" s="58"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="13"/>
@@ -3829,11 +3845,11 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B26" s="59"/>
+      <c r="B26" s="58"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="13"/>
@@ -3868,11 +3884,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C27" s="12"/>
@@ -3911,11 +3927,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C28" s="12"/>
@@ -3950,11 +3966,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="B29" s="59"/>
+      <c r="B29" s="58"/>
       <c r="C29" s="12"/>
       <c r="D29" s="15" t="s">
         <v>370</v>
@@ -3991,11 +4007,11 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="59" t="s">
+      <c r="B30" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -4038,11 +4054,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B31" s="60"/>
+      <c r="B31" s="59"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="13"/>
@@ -4077,11 +4093,11 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="B32" s="59"/>
+      <c r="B32" s="58"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="13"/>
@@ -4116,11 +4132,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="B33" s="59"/>
+      <c r="B33" s="58"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="13"/>
@@ -4155,11 +4171,11 @@
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="B34" s="59"/>
+      <c r="B34" s="58"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="13"/>
@@ -4194,11 +4210,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="B35" s="59"/>
+      <c r="B35" s="58"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="13"/>
@@ -4233,11 +4249,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="B36" s="59"/>
+      <c r="B36" s="58"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
       <c r="E36" s="13"/>
@@ -4272,11 +4288,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="B37" s="59"/>
+      <c r="B37" s="58"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
       <c r="E37" s="13"/>
@@ -4311,11 +4327,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
         <v>279</v>
       </c>
-      <c r="B38" s="60"/>
+      <c r="B38" s="59"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="13" t="s">
@@ -4352,11 +4368,11 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="B39" s="59"/>
+      <c r="B39" s="58"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="13" t="s">
@@ -4393,11 +4409,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="B40" s="59"/>
+      <c r="B40" s="58"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="13" t="s">
@@ -4434,11 +4450,11 @@
         <v>253</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="B41" s="59"/>
+      <c r="B41" s="58"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="13" t="s">
@@ -4475,11 +4491,11 @@
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="B42" s="59"/>
+      <c r="B42" s="58"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="13" t="s">
@@ -4516,11 +4532,11 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="59" t="s">
+      <c r="B43" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C43" s="12" t="s">
@@ -4567,11 +4583,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="59" t="s">
+      <c r="B44" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C44" s="12" t="s">
@@ -4614,11 +4630,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="59" t="s">
+      <c r="B45" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C45" s="12" t="s">
@@ -4665,11 +4681,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="59" t="s">
+      <c r="B46" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C46" s="12" t="s">
@@ -4714,11 +4730,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="59" t="s">
+      <c r="B47" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C47" s="12" t="s">
@@ -4763,11 +4779,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A48" s="47" t="s">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="70" t="s">
+      <c r="B48" s="69" t="s">
         <v>336</v>
       </c>
       <c r="C48" s="15" t="s">
@@ -4808,11 +4824,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="B49" s="59"/>
+      <c r="B49" s="58"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="13"/>
@@ -4843,11 +4859,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="B50" s="59" t="s">
+      <c r="B50" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C50" s="12" t="s">
@@ -4892,11 +4908,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B51" s="59" t="s">
+      <c r="B51" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C51" s="12" t="s">
@@ -4941,11 +4957,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="69" t="s">
+      <c r="B52" s="68" t="s">
         <v>351</v>
       </c>
       <c r="C52" s="12" t="s">
@@ -4990,11 +5006,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="B53" s="59"/>
+      <c r="B53" s="58"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
       <c r="E53" s="13"/>
@@ -5025,11 +5041,11 @@
         <v>273</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="59"/>
+      <c r="B54" s="58"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
       <c r="E54" s="13"/>
@@ -5058,11 +5074,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B55" s="59" t="s">
+      <c r="B55" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C55" s="12" t="s">
@@ -5109,11 +5125,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="B56" s="59" t="s">
+      <c r="B56" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C56" s="12" t="s">
@@ -5158,11 +5174,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="B57" s="59" t="s">
+      <c r="B57" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C57" s="12" t="s">
@@ -5207,11 +5223,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="59"/>
+      <c r="B58" s="58"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
       <c r="E58" s="13"/>
@@ -5240,11 +5256,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B59" s="59" t="s">
+      <c r="B59" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C59" s="12" t="s">
@@ -5287,11 +5303,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B60" s="59"/>
+      <c r="B60" s="58"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
       <c r="E60" s="13"/>
@@ -5326,11 +5342,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="B61" s="59"/>
+      <c r="B61" s="58"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
       <c r="E61" s="13"/>
@@ -5361,11 +5377,11 @@
         <v>274</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B62" s="59"/>
+      <c r="B62" s="58"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
       <c r="E62" s="13"/>
@@ -5400,11 +5416,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="B63" s="59"/>
+      <c r="B63" s="58"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="13" t="s">
@@ -5412,10 +5428,10 @@
       </c>
       <c r="F63" s="11"/>
       <c r="G63" s="15" t="s">
-        <v>361</v>
+        <v>389</v>
       </c>
       <c r="H63" s="12"/>
-      <c r="I63" s="58" t="s">
+      <c r="I63" s="57" t="s">
         <v>361</v>
       </c>
       <c r="J63" s="16" t="s">
@@ -5446,11 +5462,11 @@
         <v>185</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B64" s="59"/>
+      <c r="B64" s="58"/>
       <c r="C64" s="12"/>
       <c r="D64" s="12"/>
       <c r="E64" s="13"/>
@@ -5485,11 +5501,11 @@
         <v>158</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="B65" s="59"/>
+      <c r="B65" s="58"/>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
       <c r="E65" s="13"/>
@@ -5520,11 +5536,11 @@
         <v>271</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B66" s="59" t="s">
+      <c r="B66" s="58" t="s">
         <v>314</v>
       </c>
       <c r="C66" s="12" t="s">
@@ -5571,11 +5587,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="B67" s="59" t="s">
+      <c r="B67" s="58" t="s">
         <v>315</v>
       </c>
       <c r="C67" s="12" t="s">
@@ -5622,11 +5638,11 @@
         <v>182</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="B68" s="59" t="s">
+      <c r="B68" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C68" s="12" t="s">
@@ -5673,11 +5689,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B69" s="59" t="s">
+      <c r="B69" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C69" s="12" t="s">
@@ -5724,11 +5740,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B70" s="59"/>
+      <c r="B70" s="58"/>
       <c r="C70" s="12"/>
       <c r="D70" s="12"/>
       <c r="E70" s="13"/>
@@ -5761,11 +5777,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B71" s="59" t="s">
+      <c r="B71" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C71" s="12" t="s">
@@ -5812,11 +5828,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B72" s="62"/>
+      <c r="B72" s="61"/>
       <c r="C72" s="33"/>
       <c r="D72" s="33"/>
       <c r="E72" s="34"/>
@@ -5848,11 +5864,11 @@
       </c>
       <c r="T72" s="21"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="B73" s="59"/>
+      <c r="B73" s="58"/>
       <c r="C73" s="12"/>
       <c r="D73" s="12"/>
       <c r="E73" s="13"/>
@@ -5889,11 +5905,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="B74" s="59"/>
+      <c r="B74" s="58"/>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="13"/>
@@ -5930,11 +5946,11 @@
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="B75" s="60"/>
+      <c r="B75" s="59"/>
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>
       <c r="E75" s="13"/>
@@ -5969,11 +5985,11 @@
         <v>276</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="28" t="s">
         <v>258</v>
       </c>
-      <c r="B76" s="59"/>
+      <c r="B76" s="58"/>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
       <c r="E76" s="13"/>
@@ -6008,11 +6024,11 @@
         <v>342</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="B77" s="59"/>
+      <c r="B77" s="58"/>
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
       <c r="E77" s="13"/>
@@ -6047,11 +6063,11 @@
         <v>260</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="B78" s="59"/>
+      <c r="B78" s="58"/>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
       <c r="E78" s="13"/>
@@ -6086,11 +6102,11 @@
         <v>262</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="28" t="s">
         <v>265</v>
       </c>
-      <c r="B79" s="59"/>
+      <c r="B79" s="58"/>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
       <c r="E79" s="13"/>
@@ -6125,11 +6141,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="28" t="s">
         <v>263</v>
       </c>
-      <c r="B80" s="59"/>
+      <c r="B80" s="58"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
       <c r="E80" s="13"/>
@@ -6164,11 +6180,11 @@
         <v>264</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B81" s="60"/>
+      <c r="B81" s="59"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
       <c r="E81" s="13" t="s">
@@ -6209,15 +6225,15 @@
       <c r="S81" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="T81" s="53" t="s">
+      <c r="T81" s="52" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="B82" s="59"/>
+      <c r="B82" s="58"/>
       <c r="C82" s="12"/>
       <c r="D82" s="12"/>
       <c r="E82" s="13" t="s">
@@ -6262,11 +6278,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B83" s="59"/>
+      <c r="B83" s="58"/>
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
       <c r="E83" s="13" t="s">
@@ -6311,11 +6327,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="B84" s="59"/>
+      <c r="B84" s="58"/>
       <c r="C84" s="12"/>
       <c r="D84" s="12"/>
       <c r="E84" s="13" t="s">
@@ -6360,11 +6376,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="B85" s="59"/>
+      <c r="B85" s="58"/>
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
       <c r="E85" s="13" t="s">
@@ -6409,11 +6425,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B86" s="59"/>
+      <c r="B86" s="58"/>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
       <c r="E86" s="13" t="s">
@@ -6458,11 +6474,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="B87" s="59"/>
+      <c r="B87" s="58"/>
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
       <c r="E87" s="13" t="s">
@@ -6507,11 +6523,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="B88" s="59"/>
+      <c r="B88" s="58"/>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
       <c r="E88" s="13" t="s">
@@ -6556,11 +6572,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="B89" s="59"/>
+      <c r="B89" s="58"/>
       <c r="C89" s="12"/>
       <c r="D89" s="12"/>
       <c r="E89" s="13" t="s">
@@ -6605,11 +6621,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="B90" s="59"/>
+      <c r="B90" s="58"/>
       <c r="C90" s="12"/>
       <c r="D90" s="12"/>
       <c r="E90" s="13" t="s">
@@ -6654,11 +6670,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B91" s="59"/>
+      <c r="B91" s="58"/>
       <c r="C91" s="12"/>
       <c r="D91" s="12"/>
       <c r="E91" s="13" t="s">
@@ -6703,11 +6719,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B92" s="59"/>
+      <c r="B92" s="58"/>
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
       <c r="E92" s="13" t="s">
@@ -6752,11 +6768,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="30" t="s">
         <v>311</v>
       </c>
-      <c r="B93" s="59"/>
+      <c r="B93" s="58"/>
       <c r="C93" s="12"/>
       <c r="D93" s="12"/>
       <c r="E93" s="13" t="s">
@@ -6801,11 +6817,11 @@
         <v>82</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="30" t="s">
         <v>329</v>
       </c>
-      <c r="B94" s="59"/>
+      <c r="B94" s="58"/>
       <c r="C94" s="12"/>
       <c r="D94" s="12"/>
       <c r="E94" s="13" t="s">
@@ -6850,11 +6866,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="43" t="s">
         <v>328</v>
       </c>
-      <c r="B95" s="61"/>
+      <c r="B95" s="60"/>
       <c r="C95" s="12"/>
       <c r="D95" s="12"/>
       <c r="E95" s="13" t="s">
@@ -6899,11 +6915,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="B96" s="59"/>
+      <c r="B96" s="58"/>
       <c r="C96" s="12"/>
       <c r="D96" s="12"/>
       <c r="E96" s="13" t="s">
@@ -6948,11 +6964,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B97" s="59"/>
+      <c r="B97" s="58"/>
       <c r="C97" s="12"/>
       <c r="D97" s="12"/>
       <c r="E97" s="13" t="s">
@@ -6997,11 +7013,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B98" s="59"/>
+      <c r="B98" s="58"/>
       <c r="C98" s="12"/>
       <c r="D98" s="12"/>
       <c r="E98" s="13"/>
@@ -7038,11 +7054,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B99" s="59"/>
+      <c r="B99" s="58"/>
       <c r="C99" s="12"/>
       <c r="D99" s="12"/>
       <c r="E99" s="13" t="s">
@@ -7081,11 +7097,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B100" s="59"/>
+      <c r="B100" s="58"/>
       <c r="C100" s="12"/>
       <c r="D100" s="12"/>
       <c r="E100" s="13" t="s">
@@ -7124,13 +7140,13 @@
         <v>103</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="B101" s="71"/>
-      <c r="C101" s="72"/>
-      <c r="D101" s="73"/>
+      <c r="B101" s="70"/>
+      <c r="C101" s="71"/>
+      <c r="D101" s="72"/>
       <c r="E101" s="13" t="s">
         <v>363</v>
       </c>
@@ -7169,11 +7185,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B102" s="59"/>
+      <c r="B102" s="58"/>
       <c r="C102" s="12"/>
       <c r="D102" s="12"/>
       <c r="E102" s="13"/>
@@ -7214,11 +7230,11 @@
         <v>166</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B103" s="59"/>
+      <c r="B103" s="58"/>
       <c r="C103" s="12"/>
       <c r="D103" s="12"/>
       <c r="E103" s="13"/>
@@ -7253,11 +7269,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B104" s="59"/>
+      <c r="B104" s="58"/>
       <c r="C104" s="12"/>
       <c r="D104" s="12"/>
       <c r="E104" s="13"/>
@@ -7294,11 +7310,11 @@
         <v>108</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="B105" s="59"/>
+      <c r="B105" s="58"/>
       <c r="C105" s="12"/>
       <c r="D105" s="12"/>
       <c r="E105" s="13"/>
@@ -7333,11 +7349,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="B106" s="59"/>
+      <c r="B106" s="58"/>
       <c r="C106" s="12"/>
       <c r="D106" s="12"/>
       <c r="E106" s="13"/>
@@ -7374,11 +7390,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="B107" s="59"/>
+      <c r="B107" s="58"/>
       <c r="C107" s="12"/>
       <c r="D107" s="12"/>
       <c r="E107" s="13"/>
@@ -7415,17 +7431,19 @@
         <v>343</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B108" s="64"/>
+      <c r="B108" s="63"/>
       <c r="C108" s="37"/>
       <c r="D108" s="37"/>
-      <c r="E108" s="38"/>
+      <c r="E108" s="38" t="s">
+        <v>391</v>
+      </c>
       <c r="F108" s="36"/>
       <c r="G108" s="37" t="s">
-        <v>293</v>
+        <v>392</v>
       </c>
       <c r="H108" s="37"/>
       <c r="I108" s="37"/>
@@ -7438,7 +7456,9 @@
       <c r="N108" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="O108" s="36"/>
+      <c r="O108" s="36" t="s">
+        <v>390</v>
+      </c>
       <c r="P108" s="37" t="s">
         <v>298</v>
       </c>
@@ -7449,11 +7469,11 @@
       </c>
       <c r="T108" s="22"/>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B109" s="59"/>
+      <c r="B109" s="58"/>
       <c r="C109" s="12"/>
       <c r="D109" s="12"/>
       <c r="E109" s="13"/>
@@ -7488,11 +7508,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B110" s="59"/>
+      <c r="B110" s="58"/>
       <c r="C110" s="12"/>
       <c r="D110" s="12"/>
       <c r="E110" s="13" t="s">
@@ -7531,11 +7551,11 @@
         <v>68</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B111" s="59"/>
+      <c r="B111" s="58"/>
       <c r="C111" s="12"/>
       <c r="D111" s="12"/>
       <c r="E111" s="13" t="s">
@@ -7574,11 +7594,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B112" s="59"/>
+      <c r="B112" s="58"/>
       <c r="C112" s="12"/>
       <c r="D112" s="12"/>
       <c r="E112" s="13"/>
@@ -7613,11 +7633,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A113" s="47" t="s">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A113" s="46" t="s">
         <v>220</v>
       </c>
-      <c r="B113" s="61"/>
+      <c r="B113" s="60"/>
       <c r="C113" s="12"/>
       <c r="D113" s="12"/>
       <c r="E113" s="13"/>
@@ -7652,16 +7672,18 @@
         <v>221</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B114" s="59"/>
+      <c r="B114" s="58"/>
       <c r="C114" s="12"/>
       <c r="D114" s="12"/>
       <c r="E114" s="13"/>
       <c r="F114" s="11"/>
-      <c r="G114" s="46"/>
+      <c r="G114" s="76" t="s">
+        <v>388</v>
+      </c>
       <c r="H114" s="12"/>
       <c r="I114" s="12"/>
       <c r="J114" s="13" t="str">
@@ -7689,11 +7711,11 @@
         <v>344</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="B115" s="59"/>
+      <c r="B115" s="58"/>
       <c r="C115" s="12"/>
       <c r="D115" s="12"/>
       <c r="E115" s="13"/>
@@ -7728,11 +7750,11 @@
         <v>199</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B116" s="59"/>
+      <c r="B116" s="58"/>
       <c r="C116" s="12"/>
       <c r="D116" s="12"/>
       <c r="E116" s="13" t="s">
@@ -7771,11 +7793,11 @@
         <v>341</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A117" s="47" t="s">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A117" s="46" t="s">
         <v>330</v>
       </c>
-      <c r="B117" s="61"/>
+      <c r="B117" s="60"/>
       <c r="C117" s="12"/>
       <c r="D117" s="12"/>
       <c r="E117" s="13" t="s">
@@ -7814,11 +7836,11 @@
         <v>340</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B118" s="59"/>
+      <c r="B118" s="58"/>
       <c r="C118" s="12"/>
       <c r="D118" s="12"/>
       <c r="E118" s="13" t="s">
@@ -7855,11 +7877,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B119" s="59"/>
+      <c r="B119" s="58"/>
       <c r="C119" s="12"/>
       <c r="D119" s="12"/>
       <c r="E119" s="13" t="s">
@@ -7898,11 +7920,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A120" s="47" t="s">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A120" s="46" t="s">
         <v>331</v>
       </c>
-      <c r="B120" s="61"/>
+      <c r="B120" s="60"/>
       <c r="C120" s="12"/>
       <c r="D120" s="12"/>
       <c r="E120" s="13" t="s">
@@ -7941,11 +7963,11 @@
         <v>338</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B121" s="59"/>
+      <c r="B121" s="58"/>
       <c r="C121" s="12"/>
       <c r="D121" s="12"/>
       <c r="E121" s="13"/>
@@ -7980,11 +8002,11 @@
         <v>210</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B122" s="59"/>
+      <c r="B122" s="58"/>
       <c r="C122" s="12"/>
       <c r="D122" s="12"/>
       <c r="E122" s="13" t="s">
@@ -8023,11 +8045,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B123" s="59"/>
+      <c r="B123" s="58"/>
       <c r="C123" s="12"/>
       <c r="D123" s="12"/>
       <c r="E123" s="13"/>
@@ -8062,11 +8084,11 @@
         <v>213</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="B124" s="59"/>
+      <c r="B124" s="58"/>
       <c r="C124" s="12"/>
       <c r="D124" s="12"/>
       <c r="E124" s="13"/>
@@ -8101,11 +8123,11 @@
         <v>201</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B125" s="59"/>
+      <c r="B125" s="58"/>
       <c r="C125" s="12"/>
       <c r="D125" s="12"/>
       <c r="E125" s="13"/>
@@ -8140,11 +8162,11 @@
         <v>208</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B126" s="59"/>
+      <c r="B126" s="58"/>
       <c r="C126" s="12"/>
       <c r="D126" s="12"/>
       <c r="E126" s="13"/>
@@ -8179,11 +8201,11 @@
         <v>206</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B127" s="59"/>
+      <c r="B127" s="58"/>
       <c r="C127" s="12"/>
       <c r="D127" s="12"/>
       <c r="E127" s="13" t="s">
@@ -8222,16 +8244,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="B128" s="59"/>
+      <c r="B128" s="58"/>
       <c r="C128" s="12"/>
       <c r="D128" s="12"/>
       <c r="E128" s="13"/>
       <c r="F128" s="11"/>
-      <c r="G128" s="46"/>
+      <c r="G128" s="76" t="s">
+        <v>388</v>
+      </c>
       <c r="H128" s="12"/>
       <c r="I128" s="12"/>
       <c r="J128" s="13" t="str">
@@ -8259,11 +8283,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="B129" s="59"/>
+      <c r="B129" s="58"/>
       <c r="C129" s="12"/>
       <c r="D129" s="12"/>
       <c r="E129" s="13" t="s">
@@ -8302,11 +8326,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B130" s="59"/>
+      <c r="B130" s="58"/>
       <c r="C130" s="12"/>
       <c r="D130" s="12"/>
       <c r="E130" s="13" t="s">
@@ -8345,11 +8369,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B131" s="60"/>
+      <c r="B131" s="59"/>
       <c r="C131" s="12"/>
       <c r="D131" s="12"/>
       <c r="E131" s="13"/>
@@ -8384,11 +8408,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="B132" s="59"/>
+      <c r="B132" s="58"/>
       <c r="C132" s="12"/>
       <c r="D132" s="12"/>
       <c r="E132" s="13"/>
@@ -8423,11 +8447,11 @@
         <v>226</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="B133" s="59"/>
+      <c r="B133" s="58"/>
       <c r="C133" s="12"/>
       <c r="D133" s="12"/>
       <c r="E133" s="13"/>
@@ -8462,11 +8486,11 @@
         <v>224</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="B134" s="59"/>
+      <c r="B134" s="58"/>
       <c r="C134" s="12"/>
       <c r="D134" s="12"/>
       <c r="E134" s="13"/>
@@ -8501,11 +8525,11 @@
         <v>246</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="B135" s="59"/>
+      <c r="B135" s="58"/>
       <c r="C135" s="12"/>
       <c r="D135" s="12"/>
       <c r="E135" s="13"/>
@@ -8540,11 +8564,11 @@
         <v>228</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" s="28" t="s">
         <v>256</v>
       </c>
-      <c r="B136" s="59"/>
+      <c r="B136" s="58"/>
       <c r="C136" s="12"/>
       <c r="D136" s="12"/>
       <c r="E136" s="13"/>
@@ -8579,11 +8603,11 @@
         <v>257</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="B137" s="59"/>
+      <c r="B137" s="58"/>
       <c r="C137" s="12"/>
       <c r="D137" s="12"/>
       <c r="E137" s="13"/>
@@ -8618,11 +8642,11 @@
         <v>230</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="B138" s="59"/>
+      <c r="B138" s="58"/>
       <c r="C138" s="12"/>
       <c r="D138" s="12"/>
       <c r="E138" s="13"/>
@@ -8657,11 +8681,11 @@
         <v>231</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" s="28" t="s">
         <v>254</v>
       </c>
-      <c r="B139" s="59"/>
+      <c r="B139" s="58"/>
       <c r="C139" s="12"/>
       <c r="D139" s="12"/>
       <c r="E139" s="13"/>
@@ -8696,11 +8720,11 @@
         <v>255</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="B140" s="59"/>
+      <c r="B140" s="58"/>
       <c r="C140" s="12"/>
       <c r="D140" s="12"/>
       <c r="E140" s="13"/>
@@ -8735,11 +8759,11 @@
         <v>235</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="B141" s="59"/>
+      <c r="B141" s="58"/>
       <c r="C141" s="12"/>
       <c r="D141" s="12"/>
       <c r="E141" s="13"/>
@@ -8774,11 +8798,11 @@
         <v>233</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="B142" s="59"/>
+      <c r="B142" s="58"/>
       <c r="C142" s="12"/>
       <c r="D142" s="12"/>
       <c r="E142" s="13"/>
@@ -8813,11 +8837,11 @@
         <v>237</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="B143" s="59"/>
+      <c r="B143" s="58"/>
       <c r="C143" s="12"/>
       <c r="D143" s="12"/>
       <c r="E143" s="13"/>
@@ -8852,11 +8876,11 @@
         <v>244</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="B144" s="59"/>
+      <c r="B144" s="58"/>
       <c r="C144" s="12"/>
       <c r="D144" s="12"/>
       <c r="E144" s="13"/>
@@ -8891,11 +8915,11 @@
         <v>242</v>
       </c>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" s="28" t="s">
         <v>324</v>
       </c>
-      <c r="B145" s="59"/>
+      <c r="B145" s="58"/>
       <c r="C145" s="12"/>
       <c r="D145" s="12"/>
       <c r="E145" s="13"/>
@@ -8930,11 +8954,11 @@
         <v>238</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="B146" s="59"/>
+      <c r="B146" s="58"/>
       <c r="C146" s="12"/>
       <c r="D146" s="12"/>
       <c r="E146" s="13"/>
@@ -8969,16 +8993,18 @@
         <v>240</v>
       </c>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="B147" s="59"/>
+      <c r="B147" s="58"/>
       <c r="C147" s="12"/>
       <c r="D147" s="12"/>
       <c r="E147" s="13"/>
       <c r="F147" s="11"/>
-      <c r="G147" s="46"/>
+      <c r="G147" s="76" t="s">
+        <v>388</v>
+      </c>
       <c r="H147" s="12"/>
       <c r="I147" s="12"/>
       <c r="J147" s="13" t="str">
@@ -9006,11 +9032,11 @@
         <v>211</v>
       </c>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B148" s="59"/>
+      <c r="B148" s="58"/>
       <c r="C148" s="12"/>
       <c r="D148" s="12"/>
       <c r="E148" s="13" t="s">
@@ -9049,11 +9075,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="B149" s="59"/>
+      <c r="B149" s="58"/>
       <c r="C149" s="12"/>
       <c r="D149" s="12"/>
       <c r="E149" s="13"/>
@@ -9088,11 +9114,11 @@
         <v>251</v>
       </c>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="B150" s="59"/>
+      <c r="B150" s="58"/>
       <c r="C150" s="12"/>
       <c r="D150" s="12"/>
       <c r="E150" s="13"/>
@@ -9127,11 +9153,11 @@
         <v>223</v>
       </c>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B151" s="59"/>
+      <c r="B151" s="58"/>
       <c r="C151" s="12"/>
       <c r="D151" s="12"/>
       <c r="E151" s="13"/>
@@ -9166,11 +9192,11 @@
         <v>345</v>
       </c>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="B152" s="59"/>
+      <c r="B152" s="58"/>
       <c r="C152" s="12"/>
       <c r="D152" s="12"/>
       <c r="E152" s="13"/>
@@ -9205,11 +9231,11 @@
         <v>249</v>
       </c>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B153" s="59"/>
+      <c r="B153" s="58"/>
       <c r="C153" s="12"/>
       <c r="D153" s="12"/>
       <c r="E153" s="13" t="s">
@@ -9248,16 +9274,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B154" s="59"/>
+      <c r="B154" s="58"/>
       <c r="C154" s="12"/>
       <c r="D154" s="12"/>
       <c r="E154" s="13"/>
       <c r="F154" s="11"/>
-      <c r="G154" s="46"/>
+      <c r="G154" s="76" t="s">
+        <v>388</v>
+      </c>
       <c r="H154" s="12"/>
       <c r="I154" s="12"/>
       <c r="J154" s="13" t="str">
@@ -9285,11 +9313,11 @@
         <v>215</v>
       </c>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="B155" s="59"/>
+      <c r="B155" s="58"/>
       <c r="C155" s="12"/>
       <c r="D155" s="12"/>
       <c r="E155" s="13" t="s">
@@ -9328,11 +9356,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B156" s="59"/>
+      <c r="B156" s="58"/>
       <c r="C156" s="12"/>
       <c r="D156" s="12"/>
       <c r="E156" s="13" t="s">
@@ -9371,11 +9399,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="B157" s="59"/>
+      <c r="B157" s="58"/>
       <c r="C157" s="12"/>
       <c r="D157" s="12"/>
       <c r="E157" s="13" t="s">
@@ -9414,11 +9442,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B158" s="59"/>
+      <c r="B158" s="58"/>
       <c r="C158" s="12"/>
       <c r="D158" s="12"/>
       <c r="E158" s="13" t="s">
@@ -9457,11 +9485,11 @@
         <v>66</v>
       </c>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B159" s="59"/>
+      <c r="B159" s="58"/>
       <c r="C159" s="12"/>
       <c r="D159" s="12"/>
       <c r="E159" s="13" t="s">
@@ -9500,11 +9528,11 @@
         <v>51</v>
       </c>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A160" s="52" t="s">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A160" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B160" s="59"/>
+      <c r="B160" s="58"/>
       <c r="C160" s="12"/>
       <c r="D160" s="12"/>
       <c r="E160" s="13" t="s">
@@ -9543,11 +9571,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B161" s="59"/>
+      <c r="B161" s="58"/>
       <c r="C161" s="12"/>
       <c r="D161" s="12"/>
       <c r="E161" s="13" t="s">
@@ -9586,11 +9614,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="39" t="s">
         <v>303</v>
       </c>
-      <c r="B162" s="65"/>
+      <c r="B162" s="64"/>
       <c r="C162" s="41"/>
       <c r="D162" s="41"/>
       <c r="E162" s="42"/>
@@ -9610,11 +9638,11 @@
       <c r="S162" s="42"/>
       <c r="T162" s="23"/>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A163" s="50" t="s">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A163" s="49" t="s">
         <v>168</v>
       </c>
-      <c r="B163" s="59"/>
+      <c r="B163" s="58"/>
       <c r="C163" s="12"/>
       <c r="D163" s="12"/>
       <c r="E163" s="13"/>
@@ -9649,11 +9677,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A164" s="50" t="s">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A164" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="B164" s="59"/>
+      <c r="B164" s="58"/>
       <c r="C164" s="12"/>
       <c r="D164" s="12"/>
       <c r="E164" s="13"/>
@@ -9688,11 +9716,11 @@
         <v>175</v>
       </c>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A165" s="50" t="s">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A165" s="49" t="s">
         <v>352</v>
       </c>
-      <c r="B165" s="59" t="s">
+      <c r="B165" s="58" t="s">
         <v>363</v>
       </c>
       <c r="C165" s="12" t="s">
@@ -9745,15 +9773,15 @@
       <c r="S165" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="T165" s="54" t="s">
+      <c r="T165" s="53" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A166" s="50" t="s">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A166" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="B166" s="59"/>
+      <c r="B166" s="58"/>
       <c r="C166" s="12"/>
       <c r="D166" s="12"/>
       <c r="E166" s="13"/>
@@ -9788,11 +9816,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="B167" s="59"/>
+      <c r="B167" s="58"/>
       <c r="C167" s="12"/>
       <c r="D167" s="12"/>
       <c r="E167" s="13"/>
@@ -9821,11 +9849,11 @@
         <v>278</v>
       </c>
     </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="B168" s="59"/>
+      <c r="B168" s="58"/>
       <c r="C168" s="12"/>
       <c r="D168" s="12"/>
       <c r="E168" s="13"/>
@@ -9850,15 +9878,15 @@
       <c r="Q168" s="12"/>
       <c r="R168" s="12"/>
       <c r="S168" s="13"/>
-      <c r="T168" s="49" t="s">
+      <c r="T168" s="48" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="B169" s="59"/>
+      <c r="B169" s="58"/>
       <c r="C169" s="12"/>
       <c r="D169" s="12"/>
       <c r="E169" s="13"/>
@@ -9887,15 +9915,15 @@
       <c r="S169" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="T169" s="49" t="s">
+      <c r="T169" s="48" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A170" s="50" t="s">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A170" s="49" t="s">
         <v>178</v>
       </c>
-      <c r="B170" s="59"/>
+      <c r="B170" s="58"/>
       <c r="C170" s="12"/>
       <c r="D170" s="12"/>
       <c r="E170" s="13"/>
@@ -9930,11 +9958,11 @@
         <v>179</v>
       </c>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="B171" s="59"/>
+      <c r="B171" s="58"/>
       <c r="C171" s="12"/>
       <c r="D171" s="12"/>
       <c r="E171" s="13"/>
@@ -9965,11 +9993,11 @@
         <v>269</v>
       </c>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A172" s="50" t="s">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A172" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="B172" s="59"/>
+      <c r="B172" s="58"/>
       <c r="C172" s="12"/>
       <c r="D172" s="12"/>
       <c r="E172" s="13"/>
@@ -10051,36 +10079,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="88.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
         <v>281</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="74" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="74" t="s">
         <v>381</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="74" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="75" t="s">
         <v>308</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="75" t="s">
         <v>370</v>
       </c>
-      <c r="C2" s="76" t="str">
+      <c r="C2" s="75" t="str">
         <f>Links[[#This Row],[Feature]]&amp;":"&amp;Links[[#This Row],[Text]]</f>
         <v>Microsoft 365 Apps (Office):Business
 (No SCA)</v>
@@ -10089,14 +10117,14 @@
         <v>376</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A3" s="76" t="s">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="75" t="s">
         <v>308</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="75" t="s">
         <v>371</v>
       </c>
-      <c r="C3" s="76" t="str">
+      <c r="C3" s="75" t="str">
         <f>Links[[#This Row],[Feature]]&amp;":"&amp;Links[[#This Row],[Text]]</f>
         <v>Microsoft 365 Apps (Office):Business
 (With SCA)</v>
@@ -10105,14 +10133,14 @@
         <v>376</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="76" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="75" t="s">
         <v>308</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="75" t="s">
         <v>306</v>
       </c>
-      <c r="C4" s="76" t="str">
+      <c r="C4" s="75" t="str">
         <f>Links[[#This Row],[Feature]]&amp;":"&amp;Links[[#This Row],[Text]]</f>
         <v>Microsoft 365 Apps (Office):Enterprise</v>
       </c>
@@ -10120,14 +10148,14 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="76" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="75" t="s">
         <v>308</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="75" t="s">
         <v>307</v>
       </c>
-      <c r="C5" s="76" t="str">
+      <c r="C5" s="75" t="str">
         <f>Links[[#This Row],[Feature]]&amp;":"&amp;Links[[#This Row],[Text]]</f>
         <v>Microsoft 365 Apps (Office):Education</v>
       </c>
@@ -10135,14 +10163,14 @@
         <v>379</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="76" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="75" t="s">
         <v>336</v>
       </c>
-      <c r="C6" s="76" t="str">
+      <c r="C6" s="75" t="str">
         <f>Links[[#This Row],[Feature]]&amp;":"&amp;Links[[#This Row],[Text]]</f>
         <v>MyAnalytics:Insights</v>
       </c>
@@ -10150,14 +10178,14 @@
         <v>377</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="76" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="75" t="s">
         <v>337</v>
       </c>
-      <c r="C7" s="76" t="str">
+      <c r="C7" s="75" t="str">
         <f>Links[[#This Row],[Feature]]&amp;":"&amp;Links[[#This Row],[Text]]</f>
         <v>MyAnalytics:Full</v>
       </c>
@@ -10165,14 +10193,14 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" s="76" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="75" t="s">
         <v>360</v>
       </c>
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="75" t="s">
         <v>361</v>
       </c>
-      <c r="C8" s="76" t="str">
+      <c r="C8" s="75" t="str">
         <f>Links[[#This Row],[Feature]]&amp;":"&amp;Links[[#This Row],[Text]]</f>
         <v>Retention Labels &amp; Policies:Policies</v>
       </c>
@@ -10180,14 +10208,14 @@
         <v>378</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" s="76" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="75" t="s">
         <v>305</v>
       </c>
-      <c r="B9" s="76" t="s">
+      <c r="B9" s="75" t="s">
         <v>307</v>
       </c>
-      <c r="C9" s="76" t="str">
+      <c r="C9" s="75" t="str">
         <f>Links[[#This Row],[Feature]]&amp;":"&amp;Links[[#This Row],[Text]]</f>
         <v>Intune:Education</v>
       </c>
@@ -10197,9 +10225,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>